<commit_message>
update example for snowball to use DCF
</commit_message>
<xml_diff>
--- a/miscs/excel/005.snowball.xlsx
+++ b/miscs/excel/005.snowball.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\dal\miscs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98ACAA9-4D23-425C-BE96-D5286E9E138B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0DDC7C-7576-449C-B6F9-FEE7C9B826D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A658F64F-54DB-47F5-8888-F8582537DD58}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>spot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,10 +84,6 @@
   </si>
   <si>
     <t>repo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alive=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -117,9 +113,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.000000_ ;_ * \-#,##0.000000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +148,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -187,7 +191,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -197,9 +201,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -229,6 +230,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -549,496 +559,461 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.625" customWidth="1"/>
-    <col min="2" max="2" width="58.75" style="6" customWidth="1"/>
+    <col min="2" max="2" width="103.25" style="5" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
     <col min="4" max="4" width="73.875" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7">
+      <c r="B1" s="6">
         <v>44986</v>
       </c>
+      <c r="D1" t="str">
+        <f ca="1">TEXT(B1,"yyyy-mm-dd")</f>
+        <v>2023-03-01</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" cm="1">
+      <c r="B2" s="13" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_xll.EVALUATIONDATE.SET(B1)</f>
         <v>44986</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">_xll.BSMODELDATA.NEW("model",B4,B7,B5,B6)</f>
-        <v>~BSModelData_~model~000002599A0FE980</v>
+        <v>~BSModelData_~model~000001E64D9D0C60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0</v>
       </c>
       <c r="D5" t="str" cm="1">
-        <f t="array" aca="1" ref="D5" ca="1">_xll.PRODUCT.NEW("my_product",A16:A40,B16:B40)</f>
-        <v>~ScriptProduct~my_product~00000259881740C0</v>
+        <f t="array" aca="1" ref="D5" ca="1">_xll.PRODUCT.NEW("my_product",A16:A37,B16:B37)</f>
+        <v>~ScriptProduct~my_product~000001EE54B1A9C0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.15</v>
       </c>
-      <c r="D7" s="11" t="str" cm="1">
-        <f t="array" aca="1" ref="D7:E11" ca="1">_xll.MONTECARLO.VALUE('script（snowball）'!D5,D4,2^20,"sobol",FALSE,TRUE,0.01)</f>
+      <c r="D7" s="10" t="str" cm="1">
+        <f t="array" aca="1" ref="D7:E11" ca="1">_xll.MONTECARLO.VALUE('script（snowball）'!D5,D4,500000,"sobol",FALSE,TRUE,0.01)</f>
         <v>d_div</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="14">
         <f ca="1"/>
-        <v>-0.61848778929262194</v>
+        <v>-0.62739378949553548</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="9"/>
-      <c r="D8" s="11" t="str">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8"/>
+      <c r="D8" s="10" t="str">
         <f ca="1"/>
         <v>d_rate</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="14">
         <f ca="1"/>
-        <v>0.6826452523259382</v>
+        <v>0.69164023415199172</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>8</v>
+      <c r="A9" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="11" t="str">
+      <c r="D9" s="10" t="str">
         <f ca="1"/>
         <v>d_spot</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="14">
         <f ca="1"/>
-        <v>0.49587819300664837</v>
+        <v>0.49883293381134147</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
+      <c r="A10" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>0.88</v>
       </c>
-      <c r="D10" s="11" t="str">
+      <c r="D10" s="10" t="str">
         <f ca="1"/>
         <v>d_vol</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="14">
         <f ca="1"/>
-        <v>-0.2952963850726002</v>
+        <v>-0.29567175734222889</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10">
+      <c r="A11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="D11" s="11" t="str">
+      <c r="D11" s="10" t="str">
         <f ca="1"/>
         <v>value</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="14">
         <f ca="1"/>
-        <v>-1.4237319220099021E-2</v>
+        <v>-1.428669039549393E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>11</v>
+      <c r="C15" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <f ca="1">B2</f>
         <v>44986</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5">
-        <f ca="1">$B$11*(A16-$B$1)/365</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>45017</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="5">
-        <f t="shared" ref="C17:C40" ca="1" si="0">$B$11*(A17-$B$1)/365</f>
-        <v>5.8602739726027406E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>45047</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.153150684931507E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>45078</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.7391780821917811E-2</v>
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>45108</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <f ca="1">"if spot() &lt; "&amp;$B$10&amp;":0.001 then knock_in = 1 endif"&amp;CHAR(10)&amp;"if spot() &gt; "&amp;$B$9&amp;":0.001 then call pays alive * "&amp;TEXT(C17, "0.000000")&amp;" alive = 0  endif"</f>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2023-07-01) alive = 0  endif</v>
+      </c>
+      <c r="C17" s="15" t="str">
+        <f ca="1">TEXT($B$11,"0.000000")&amp;" * DCF(ACT365F,  "&amp;TEXT($B$2,"yyyy-mm-dd")&amp;", "&amp;TEXT(A17,"yyyy-mm-dd")&amp;")"</f>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2023-07-01)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>45139</v>
+      </c>
+      <c r="B18" s="5" t="str">
+        <f t="shared" ref="B18:B36" ca="1" si="0">"if spot() &lt; "&amp;$B$10&amp;":0.001 then knock_in = 1 endif"&amp;CHAR(10)&amp;"if spot() &gt; "&amp;$B$9&amp;":0.001 then call pays alive * "&amp;TEXT(C18, "0.0000")&amp;" alive = 0  endif"</f>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2023-08-01) alive = 0  endif</v>
+      </c>
+      <c r="C18" s="15" t="str">
+        <f t="shared" ref="C18:C37" ca="1" si="1">TEXT($B$11,"0.000000")&amp;" * DCF(ACT365F,  "&amp;TEXT($B$2,"yyyy-mm-dd")&amp;", "&amp;TEXT(A18,"yyyy-mm-dd")&amp;")"</f>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2023-08-01)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>45170</v>
+      </c>
+      <c r="B19" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2023-09-01) alive = 0  endif</v>
+      </c>
+      <c r="C19" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2023-09-01)</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>45108</v>
-      </c>
-      <c r="B20" s="6" t="str">
-        <f ca="1">"if spot() &lt; "&amp;$B$10&amp;":0.001 then knock_in = 1 endif"&amp;CHAR(10)&amp;"if spot() &gt; "&amp;$B$9&amp;":0.001 then call pays alive * "&amp;TEXT(C20, "0.0000")&amp;" alive = 0  endif"</f>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0231 alive = 0  endif</v>
-      </c>
-      <c r="C20" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.306301369863014E-2</v>
+      <c r="A20" s="3">
+        <v>45200</v>
+      </c>
+      <c r="B20" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2023-10-01) alive = 0  endif</v>
+      </c>
+      <c r="C20" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2023-10-01)</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>45139</v>
-      </c>
-      <c r="B21" s="6" t="str">
-        <f t="shared" ref="B21:B39" ca="1" si="1">"if spot() &lt; "&amp;$B$10&amp;":0.001 then knock_in = 1 endif"&amp;CHAR(10)&amp;"if spot() &gt; "&amp;$B$9&amp;":0.001 then call pays alive * "&amp;TEXT(C21, "0.0000")&amp;" alive = 0  endif"</f>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0289 alive = 0  endif</v>
-      </c>
-      <c r="C21" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.8923287671232877E-2</v>
+      <c r="A21" s="3">
+        <v>45231</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2023-11-01) alive = 0  endif</v>
+      </c>
+      <c r="C21" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2023-11-01)</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>45170</v>
-      </c>
-      <c r="B22" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0348 alive = 0  endif</v>
-      </c>
-      <c r="C22" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.4783561643835621E-2</v>
+      <c r="A22" s="3">
+        <v>45261</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2023-12-01) alive = 0  endif</v>
+      </c>
+      <c r="C22" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2023-12-01)</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>45200</v>
-      </c>
-      <c r="B23" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0405 alive = 0  endif</v>
-      </c>
-      <c r="C23" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.0454794520547947E-2</v>
+      <c r="A23" s="3">
+        <v>45292</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-01-01) alive = 0  endif</v>
+      </c>
+      <c r="C23" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-01-01)</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>45231</v>
-      </c>
-      <c r="B24" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0463 alive = 0  endif</v>
-      </c>
-      <c r="C24" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.6315068493150688E-2</v>
+      <c r="A24" s="3">
+        <v>45323</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-02-01) alive = 0  endif</v>
+      </c>
+      <c r="C24" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-02-01)</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>45261</v>
-      </c>
-      <c r="B25" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0520 alive = 0  endif</v>
-      </c>
-      <c r="C25" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1986301369863021E-2</v>
+      <c r="A25" s="3">
+        <v>45352</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-03-01) alive = 0  endif</v>
+      </c>
+      <c r="C25" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-03-01)</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>45292</v>
-      </c>
-      <c r="B26" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0578 alive = 0  endif</v>
-      </c>
-      <c r="C26" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.7846575342465754E-2</v>
+      <c r="A26" s="3">
+        <v>45383</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-04-01) alive = 0  endif</v>
+      </c>
+      <c r="C26" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-04-01)</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>45323</v>
-      </c>
-      <c r="B27" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0637 alive = 0  endif</v>
-      </c>
-      <c r="C27" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.3706849315068509E-2</v>
+      <c r="A27" s="3">
+        <v>45413</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-05-01) alive = 0  endif</v>
+      </c>
+      <c r="C27" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-05-01)</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>45352</v>
-      </c>
-      <c r="B28" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0692 alive = 0  endif</v>
-      </c>
-      <c r="C28" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6.9189041095890413E-2</v>
+      <c r="A28" s="3">
+        <v>45444</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-06-01) alive = 0  endif</v>
+      </c>
+      <c r="C28" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-06-01)</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>45383</v>
-      </c>
-      <c r="B29" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0750 alive = 0  endif</v>
-      </c>
-      <c r="C29" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.5049315068493147E-2</v>
+      <c r="A29" s="3">
+        <v>45474</v>
+      </c>
+      <c r="B29" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-07-01) alive = 0  endif</v>
+      </c>
+      <c r="C29" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-07-01)</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>45413</v>
-      </c>
-      <c r="B30" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0807 alive = 0  endif</v>
-      </c>
-      <c r="C30" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.0720547945205487E-2</v>
+      <c r="A30" s="3">
+        <v>45505</v>
+      </c>
+      <c r="B30" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-08-01) alive = 0  endif</v>
+      </c>
+      <c r="C30" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-08-01)</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
-        <v>45444</v>
-      </c>
-      <c r="B31" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0866 alive = 0  endif</v>
-      </c>
-      <c r="C31" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>8.6580821917808234E-2</v>
+      <c r="A31" s="3">
+        <v>45536</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-09-01) alive = 0  endif</v>
+      </c>
+      <c r="C31" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-09-01)</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
-        <v>45474</v>
-      </c>
-      <c r="B32" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0923 alive = 0  endif</v>
-      </c>
-      <c r="C32" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.225205479452056E-2</v>
+      <c r="A32" s="3">
+        <v>45566</v>
+      </c>
+      <c r="B32" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-10-01) alive = 0  endif</v>
+      </c>
+      <c r="C32" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-10-01)</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
-        <v>45505</v>
-      </c>
-      <c r="B33" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.0981 alive = 0  endif</v>
-      </c>
-      <c r="C33" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9.8112328767123294E-2</v>
+      <c r="A33" s="3">
+        <v>45597</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-11-01) alive = 0  endif</v>
+      </c>
+      <c r="C33" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-11-01)</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
-        <v>45536</v>
-      </c>
-      <c r="B34" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.1040 alive = 0  endif</v>
-      </c>
-      <c r="C34" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.10397260273972604</v>
+      <c r="A34" s="3">
+        <v>45627</v>
+      </c>
+      <c r="B34" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2024-12-01) alive = 0  endif</v>
+      </c>
+      <c r="C34" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2024-12-01)</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
-        <v>45566</v>
-      </c>
-      <c r="B35" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.1096 alive = 0  endif</v>
-      </c>
-      <c r="C35" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.10964383561643837</v>
+      <c r="A35" s="3">
+        <v>45658</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2025-01-01) alive = 0  endif</v>
+      </c>
+      <c r="C35" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2025-01-01)</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
-        <v>45597</v>
-      </c>
-      <c r="B36" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.1155 alive = 0  endif</v>
-      </c>
-      <c r="C36" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.11550410958904112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
-        <v>45627</v>
-      </c>
-      <c r="B37" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.1212 alive = 0  endif</v>
-      </c>
-      <c r="C37" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12117534246575344</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>45658</v>
-      </c>
-      <c r="B38" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.1270 alive = 0  endif</v>
-      </c>
-      <c r="C38" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12703561643835617</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
+      <c r="A36" s="3">
         <v>45689</v>
       </c>
-      <c r="B39" s="6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.1329 alive = 0  endif</v>
-      </c>
-      <c r="C39" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.13289589041095892</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
+      <c r="B36" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2025-02-01) alive = 0  endif</v>
+      </c>
+      <c r="C36" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2025-02-01)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>45717</v>
       </c>
-      <c r="B40" s="6" t="str">
-        <f ca="1">"if spot() &lt; "&amp;$B$10&amp;":0.001 then knock_in = 1 endif"&amp;CHAR(10)&amp;"if spot() &gt; "&amp;$B$9&amp;":0.001 then call pays alive * "&amp;TEXT(C40, "0.0000")&amp;" alive = 0  endif"&amp;CHAR(10)&amp;"call pays alive * knock_in * (spot() - " &amp; TEXT(B4,"0.0000") &amp; ")"</f>
-        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
-if spot() &gt; 1:0.001 then call pays alive * 0.1382 alive = 0  endif
+      <c r="B37" s="5" t="str">
+        <f ca="1">"if spot() &lt; "&amp;$B$10&amp;":0.001 then knock_in = 1 endif"&amp;CHAR(10)&amp;"if spot() &gt; "&amp;$B$9&amp;":0.001 then call pays alive * "&amp;TEXT(C37, "0.0000")&amp;" alive = 0  endif"&amp;CHAR(10)&amp;"call pays alive * knock_in * (spot() - " &amp; TEXT(B4,"0.0000") &amp; ")"</f>
+        <v>if spot() &lt; 0.88:0.001 then knock_in = 1 endif
+if spot() &gt; 1:0.001 then call pays alive * 0.069000 * DCF(ACT365F,  2023-03-01, 2025-03-01) alive = 0  endif
 call pays alive * knock_in * (spot() - 1.0000)</v>
       </c>
-      <c r="C40" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.13818904109589042</v>
+      <c r="C37" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.069000 * DCF(ACT365F,  2023-03-01, 2025-03-01)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>